<commit_message>
- Optimized test cases for expressions
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_json_expression.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_json_expression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nexial-project\git\nexial-core\src\test\resources\unittesting\artifact\script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B8233E3C-55D7-46CC-9910-9B1492D8441F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4005CCC7-94AD-4BBC-93EA-A519DD9F4E5D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="9420" tabRatio="387" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="9420" tabRatio="387" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="716">
   <si>
     <t>target</t>
   </si>
@@ -3127,17 +3127,105 @@
   ]
 }</t>
   </si>
+  <si>
+    <t>Setup</t>
+  </si>
+  <si>
+    <t>json.initial</t>
+  </si>
+  <si>
+    <t>{ "name": "Me and Myself", "data1": "", "data2": null }</t>
+  </si>
+  <si>
+    <t>Pack</t>
+  </si>
+  <si>
+    <t>{
+  "name": "Me and Myself",
+  "data1": ""
+}</t>
+  </si>
+  <si>
+    <t>[JSON(${json.initial}) =&gt; pack]</t>
+  </si>
+  <si>
+    <t>{"name":"Me and Myself","data1":""}</t>
+  </si>
+  <si>
+    <t>[JSON(${json.initial}) =&gt; compact(false)]</t>
+  </si>
+  <si>
+    <t>{"name":"Me and Myself"}</t>
+  </si>
+  <si>
+    <t>[JSON(${json.initial}) =&gt; compact(true)]</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>[JSON(${json.initial}) =&gt; addOrReplace( ,address: ["Aliso Viejo\, CA"\,"Universal City\, CA"]) compact(true) extract(address) list size]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Compact </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(removeEmpty = false)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Compact </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(removeEmpty = true)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3223,6 +3311,31 @@
       <name val="Consolas"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -3285,73 +3398,57 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3363,15 +3460,35 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3382,82 +3499,149 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -11306,24 +11490,24 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N101:N300">
-    <cfRule type="beginsWith" dxfId="26" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="29" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N101,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="25" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="28" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N101,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="27" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N101,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1 N3:N100 N301:N1048576">
-    <cfRule type="beginsWith" dxfId="23" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="26" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="5" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="25" priority="5" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="21" priority="6" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="24" priority="6" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16623,24 +16807,24 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N101:N300">
-    <cfRule type="beginsWith" dxfId="20" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="23" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N101,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="22" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N101,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="21" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N101,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1 N3:N100 N301:N1048576">
-    <cfRule type="beginsWith" dxfId="17" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="20" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="5" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="19" priority="5" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="15" priority="6" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="18" priority="6" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16660,10 +16844,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
@@ -21876,24 +22060,24 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N3:N300">
-    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="17" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N3,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="16" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N3,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="12" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="15" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N3,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1 N301:N1048576">
-    <cfRule type="beginsWith" dxfId="11" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="14" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="10" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="13" priority="10" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="9" priority="12" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="12" priority="12" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21913,10 +22097,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O304"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
@@ -21968,7 +22152,7 @@
       <c r="N1" s="42"/>
       <c r="O1" s="43"/>
     </row>
-    <row r="2" spans="1:15" ht="93" customHeight="1">
+    <row r="2" spans="1:15" ht="49.5" customHeight="1">
       <c r="A2" s="44" t="s">
         <v>537</v>
       </c>
@@ -22681,7 +22865,7 @@
       <c r="E29" s="22" t="s">
         <v>605</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="F29" s="59" t="s">
         <v>613</v>
       </c>
       <c r="G29" s="22"/>
@@ -22705,7 +22889,7 @@
       <c r="D30" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="59" t="s">
         <v>649</v>
       </c>
       <c r="F30" s="22" t="s">
@@ -23426,90 +23610,142 @@
       <c r="N57" s="19"/>
       <c r="O57" s="18"/>
     </row>
-    <row r="58" spans="1:15" ht="23.1" customHeight="1">
-      <c r="A58" s="15"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="22"/>
-      <c r="H58" s="22"/>
-      <c r="I58" s="22"/>
-      <c r="J58" s="23"/>
-      <c r="K58" s="18"/>
-      <c r="L58" s="19"/>
-      <c r="M58" s="17"/>
-      <c r="N58" s="19"/>
-      <c r="O58" s="18"/>
-    </row>
-    <row r="59" spans="1:15" ht="23.1" customHeight="1">
-      <c r="A59" s="15"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
-      <c r="I59" s="22"/>
-      <c r="J59" s="23"/>
-      <c r="K59" s="18"/>
-      <c r="L59" s="19"/>
-      <c r="M59" s="17"/>
-      <c r="N59" s="19"/>
-      <c r="O59" s="18"/>
-    </row>
-    <row r="60" spans="1:15" ht="23.1" customHeight="1">
-      <c r="A60" s="15"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="21"/>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="22"/>
-      <c r="H60" s="22"/>
-      <c r="I60" s="22"/>
-      <c r="J60" s="23"/>
-      <c r="K60" s="18"/>
-      <c r="L60" s="19"/>
-      <c r="M60" s="17"/>
-      <c r="N60" s="19"/>
-      <c r="O60" s="18"/>
-    </row>
-    <row r="61" spans="1:15" ht="23.1" customHeight="1">
-      <c r="A61" s="15"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="21"/>
-      <c r="D61" s="22"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="22"/>
-      <c r="G61" s="22"/>
-      <c r="H61" s="22"/>
-      <c r="I61" s="22"/>
-      <c r="J61" s="23"/>
-      <c r="K61" s="18"/>
-      <c r="L61" s="19"/>
-      <c r="M61" s="17"/>
-      <c r="N61" s="19"/>
-      <c r="O61" s="18"/>
-    </row>
-    <row r="62" spans="1:15" ht="23.1" customHeight="1">
-      <c r="A62" s="15"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="22"/>
-      <c r="E62" s="22"/>
-      <c r="F62" s="22"/>
-      <c r="G62" s="22"/>
-      <c r="H62" s="22"/>
-      <c r="I62" s="22"/>
-      <c r="J62" s="23"/>
-      <c r="K62" s="18"/>
-      <c r="L62" s="19"/>
-      <c r="M62" s="17"/>
-      <c r="N62" s="19"/>
-      <c r="O62" s="18"/>
+    <row r="58" spans="1:15" s="56" customFormat="1" ht="23.1" customHeight="1">
+      <c r="A58" s="48" t="s">
+        <v>702</v>
+      </c>
+      <c r="B58" s="48" t="s">
+        <v>702</v>
+      </c>
+      <c r="C58" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="51" t="s">
+        <v>319</v>
+      </c>
+      <c r="E58" s="52" t="s">
+        <v>703</v>
+      </c>
+      <c r="F58" s="51" t="s">
+        <v>704</v>
+      </c>
+      <c r="G58" s="51"/>
+      <c r="H58" s="51"/>
+      <c r="I58" s="51"/>
+      <c r="J58" s="51"/>
+      <c r="K58" s="53"/>
+      <c r="L58" s="54"/>
+      <c r="M58" s="55"/>
+      <c r="N58" s="54"/>
+      <c r="O58" s="53"/>
+    </row>
+    <row r="59" spans="1:15" s="56" customFormat="1" ht="60">
+      <c r="A59" s="48" t="s">
+        <v>705</v>
+      </c>
+      <c r="B59" s="48" t="s">
+        <v>705</v>
+      </c>
+      <c r="C59" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="E59" s="57" t="s">
+        <v>706</v>
+      </c>
+      <c r="F59" s="51" t="s">
+        <v>707</v>
+      </c>
+      <c r="G59" s="51"/>
+      <c r="H59" s="51"/>
+      <c r="I59" s="51"/>
+      <c r="J59" s="51"/>
+      <c r="K59" s="53"/>
+      <c r="L59" s="54"/>
+      <c r="M59" s="55"/>
+      <c r="N59" s="54"/>
+      <c r="O59" s="53"/>
+    </row>
+    <row r="60" spans="1:15" s="56" customFormat="1" ht="23.1" customHeight="1">
+      <c r="A60" s="48"/>
+      <c r="B60" s="49" t="s">
+        <v>714</v>
+      </c>
+      <c r="C60" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="E60" s="57" t="s">
+        <v>708</v>
+      </c>
+      <c r="F60" s="51" t="s">
+        <v>709</v>
+      </c>
+      <c r="G60" s="58"/>
+      <c r="H60" s="51"/>
+      <c r="I60" s="51"/>
+      <c r="J60" s="51"/>
+      <c r="K60" s="53"/>
+      <c r="L60" s="54"/>
+      <c r="M60" s="55"/>
+      <c r="N60" s="54"/>
+      <c r="O60" s="53"/>
+    </row>
+    <row r="61" spans="1:15" s="56" customFormat="1" ht="23.1" customHeight="1">
+      <c r="A61" s="48"/>
+      <c r="B61" s="49" t="s">
+        <v>715</v>
+      </c>
+      <c r="C61" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="E61" s="51" t="s">
+        <v>710</v>
+      </c>
+      <c r="F61" s="51" t="s">
+        <v>711</v>
+      </c>
+      <c r="G61" s="51"/>
+      <c r="H61" s="51"/>
+      <c r="I61" s="51"/>
+      <c r="J61" s="51"/>
+      <c r="K61" s="53"/>
+      <c r="L61" s="54"/>
+      <c r="M61" s="55"/>
+      <c r="N61" s="54"/>
+      <c r="O61" s="53"/>
+    </row>
+    <row r="62" spans="1:15" s="56" customFormat="1" ht="23.1" customHeight="1">
+      <c r="A62" s="48"/>
+      <c r="B62" s="49"/>
+      <c r="C62" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="E62" s="51" t="s">
+        <v>712</v>
+      </c>
+      <c r="F62" s="51" t="s">
+        <v>713</v>
+      </c>
+      <c r="G62" s="51"/>
+      <c r="H62" s="51"/>
+      <c r="I62" s="51"/>
+      <c r="J62" s="51"/>
+      <c r="K62" s="53"/>
+      <c r="L62" s="54"/>
+      <c r="M62" s="55"/>
+      <c r="N62" s="54"/>
+      <c r="O62" s="53"/>
     </row>
     <row r="63" spans="1:15" ht="23.1" customHeight="1">
       <c r="A63" s="15"/>
@@ -27620,46 +27856,58 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N5:N7">
-    <cfRule type="beginsWith" dxfId="8" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="11" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N5,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="7" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="10" priority="5" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N5,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="9" priority="6" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N5,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N104:N303">
-    <cfRule type="beginsWith" dxfId="5" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="8" priority="7" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N104,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="5" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="7" priority="8" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N104,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="6" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="6" priority="9" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N104,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1 N3:N4 N8:N103 N304:N1048576">
-    <cfRule type="beginsWith" dxfId="2" priority="7" stopIfTrue="1" operator="beginsWith" text="WARN">
+  <conditionalFormatting sqref="N1 N3:N4 N8:N57 N304:N1048576 N63:N103">
+    <cfRule type="beginsWith" dxfId="5" priority="10" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="8" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="4" priority="11" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="9" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="3" priority="12" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N58:N62">
+    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+      <formula>LEFT(N58,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+      <formula>LEFT(N58,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+      <formula>LEFT(N58,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C53 C57 C5:C6 C7:C8 C9:C10 C11:C47 C48:C49 C50:C52 C54:C55 C58:C303" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C55 C57:C303" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D53 D57 D5:D6 D7:D8 D9:D10 D11:D47 D48:D49 D50:D52 D54:D55 D58:D303" xr:uid="{00000000-0002-0000-0400-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D55 D57:D303" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>